<commit_message>
Modeling files. Use "Modeling and Control of a BallBot.pdf".
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cost" sheetId="1" r:id="rId1"/>
+    <sheet name="PCB Components" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="170">
   <si>
     <t>Motor 24V</t>
   </si>
@@ -99,13 +100,448 @@
   </si>
   <si>
     <t>TIỀN LÀM BALLBOT</t>
+  </si>
+  <si>
+    <t>2 heatsink</t>
+  </si>
+  <si>
+    <t>Đặt PCB Kha Thành</t>
+  </si>
+  <si>
+    <t>1 board</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>LibRef</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Buz</t>
+  </si>
+  <si>
+    <t>BUZZER SMD</t>
+  </si>
+  <si>
+    <t>100nF-10%</t>
+  </si>
+  <si>
+    <t>Non-Polarized Capacitor</t>
+  </si>
+  <si>
+    <t>C1, C5, C6, C7, C8, C9, C10</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>100nF-50V-C0805</t>
+  </si>
+  <si>
+    <t>3.3µF</t>
+  </si>
+  <si>
+    <t>Tantalum Capacitor</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>SM/C_ALU_SA</t>
+  </si>
+  <si>
+    <t>4.7uF-25V-Tantalum</t>
+  </si>
+  <si>
+    <t>330uF/35V</t>
+  </si>
+  <si>
+    <t>CAP ALUM 330UF 20% 35V SMD</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Size G</t>
+  </si>
+  <si>
+    <t>C_ALU_330uF_35V</t>
+  </si>
+  <si>
+    <t>220uF-6.3V</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>SM/C_ALU_SD8</t>
+  </si>
+  <si>
+    <t>220uF-6.3V-Tantalum</t>
+  </si>
+  <si>
+    <t>10nF-10%</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>10nF-50V-C0805</t>
+  </si>
+  <si>
+    <t>SS34</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 1A DO214AC</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D10, D11, D12, D13</t>
+  </si>
+  <si>
+    <t>DO-214AC (SMA)</t>
+  </si>
+  <si>
+    <t>Diode_SS14</t>
+  </si>
+  <si>
+    <t>SS14</t>
+  </si>
+  <si>
+    <t>D6, D7, D8, D9, D14, D15, D16, D17</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>FUSE</t>
+  </si>
+  <si>
+    <t>Heatsink TO220</t>
+  </si>
+  <si>
+    <t>Heatsink-231625W T?n nhi?t Nhôm ki?u TO-220 / Multiwatt, 23x16x25mm</t>
+  </si>
+  <si>
+    <t>H1, H2</t>
+  </si>
+  <si>
+    <t>HEATSINK TO-220</t>
+  </si>
+  <si>
+    <t>10uH/2A</t>
+  </si>
+  <si>
+    <t>10uH/2A ±20% SMD 6.7x6.7x4mm Inductor</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L6D38</t>
+  </si>
+  <si>
+    <t>L6D38-100M</t>
+  </si>
+  <si>
+    <t>LED SMD</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9, LED10, LED11</t>
+  </si>
+  <si>
+    <t>SM-LED-0805-Blue</t>
+  </si>
+  <si>
+    <t>LED-SMD-0805</t>
+  </si>
+  <si>
+    <t>Domino 2</t>
+  </si>
+  <si>
+    <t>Domino, 2-Pin</t>
+  </si>
+  <si>
+    <t>P1, P2A, P2B</t>
+  </si>
+  <si>
+    <t>DOMINO 2- 5mm</t>
+  </si>
+  <si>
+    <t>Header 2X10</t>
+  </si>
+  <si>
+    <t>Header, 10-Pin, Dual row</t>
+  </si>
+  <si>
+    <t>P3, P4</t>
+  </si>
+  <si>
+    <t>Header 8H</t>
+  </si>
+  <si>
+    <t>Header, 8-Pin, Right Angle</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>JP8H</t>
+  </si>
+  <si>
+    <t>Domino 4</t>
+  </si>
+  <si>
+    <t>Domino 4-Pin</t>
+  </si>
+  <si>
+    <t>P6, P7</t>
+  </si>
+  <si>
+    <t>DOMINO 4 -5mm</t>
+  </si>
+  <si>
+    <t>Header 1X3</t>
+  </si>
+  <si>
+    <t>Header, 3-Pin</t>
+  </si>
+  <si>
+    <t>P8, P9</t>
+  </si>
+  <si>
+    <t>SW?</t>
+  </si>
+  <si>
+    <t>Push SW 8x8 mm latching ON/OFF</t>
+  </si>
+  <si>
+    <t>PushSWtme1</t>
+  </si>
+  <si>
+    <t>PUSH SW</t>
+  </si>
+  <si>
+    <t>PushSWtme</t>
+  </si>
+  <si>
+    <t>NPN Transistor</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SC-43-BCE</t>
+  </si>
+  <si>
+    <t>10k-5%</t>
+  </si>
+  <si>
+    <t>RES 10k OHM 1/8W 5% 0805 SMD</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R0805</t>
+  </si>
+  <si>
+    <t>10k-5%-R0805</t>
+  </si>
+  <si>
+    <t>3.3k-5%</t>
+  </si>
+  <si>
+    <t>RES 3.3k OHM 1/8W 5% 0805 SMD</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>3.3k-5%-R0805</t>
+  </si>
+  <si>
+    <t>1.5k-5%</t>
+  </si>
+  <si>
+    <t>RES 1.5k OHM 1/8W 5% 0805 SMD</t>
+  </si>
+  <si>
+    <t>R3, R18, R21</t>
+  </si>
+  <si>
+    <t>1.5k-5%-R0805</t>
+  </si>
+  <si>
+    <t>560k-5%</t>
+  </si>
+  <si>
+    <t>RES 560k OHM 1/10W 5% 0603 SMD</t>
+  </si>
+  <si>
+    <t>R4, R16, R19, R22</t>
+  </si>
+  <si>
+    <t>560k-5%-R0603</t>
+  </si>
+  <si>
+    <t>220R-5%</t>
+  </si>
+  <si>
+    <t>RES 220 OHM 1/8W 5% 0805 SMD</t>
+  </si>
+  <si>
+    <t>R5, R17, R20, R23</t>
+  </si>
+  <si>
+    <t>220R-5%-R0805</t>
+  </si>
+  <si>
+    <t>100k-5%</t>
+  </si>
+  <si>
+    <t>RES 100k OHM 1/8W 5% 0805 SMD</t>
+  </si>
+  <si>
+    <t>R6, R11, R12, R13, R14, R24, R25, R26, R27</t>
+  </si>
+  <si>
+    <t>100k-5%-R0805</t>
+  </si>
+  <si>
+    <t>12k-5%</t>
+  </si>
+  <si>
+    <t>RES 12k OHM 1/8W 5% 0805 SMD</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>12k-5%-R0805</t>
+  </si>
+  <si>
+    <t>1k-5%</t>
+  </si>
+  <si>
+    <t>RES 1k OHM 1/8W 5% 0805 SMD</t>
+  </si>
+  <si>
+    <t>R8, R9</t>
+  </si>
+  <si>
+    <t>1k-5%-R0805</t>
+  </si>
+  <si>
+    <t>0.56R-1%</t>
+  </si>
+  <si>
+    <t>RES 0.56 OHM 1/10W 1% 0603 SMD</t>
+  </si>
+  <si>
+    <t>R10, R15, R28, R29</t>
+  </si>
+  <si>
+    <t>0.56R-1%-R0603</t>
+  </si>
+  <si>
+    <t>Test Point</t>
+  </si>
+  <si>
+    <t>TP1, TP2</t>
+  </si>
+  <si>
+    <t>Hole 1.5mm</t>
+  </si>
+  <si>
+    <t>TPS54xx</t>
+  </si>
+  <si>
+    <t>IC REG BUCK ADJ 1A 8SOIC</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SOIC-8 POWERPAD</t>
+  </si>
+  <si>
+    <t>LM1117-3.3V</t>
+  </si>
+  <si>
+    <t>800mA Low-Dropout Linear Regulator</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SOT223-4N</t>
+  </si>
+  <si>
+    <t>LMV358IDGKR</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>MSOP-8</t>
+  </si>
+  <si>
+    <t>L298</t>
+  </si>
+  <si>
+    <t>Dual Full-H Driver</t>
+  </si>
+  <si>
+    <t>U4, U5</t>
+  </si>
+  <si>
+    <t>DIP15SL2</t>
+  </si>
+  <si>
+    <t>7400</t>
+  </si>
+  <si>
+    <t>Quad 2-Input NAND Gate</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SO14-150mil</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,13 +562,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -175,23 +623,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,17 +929,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -491,208 +948,1042 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <f>SUM(D5:D47)</f>
-        <v>1226000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3">
-        <f>D5+D6+D7+D8+D12</f>
-        <v>666000</v>
+      <c r="G2" s="2">
+        <f>D5+D6+D7+D8+D12+D14</f>
+        <v>928000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3">
-        <f>D9+D10+D11</f>
-        <v>560000</v>
+      <c r="G3" s="2">
+        <f>D9+D10+D11+D13</f>
+        <v>572000</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>300000</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>160000</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>100000</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>70000</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="3" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>30000</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>140000</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>390000</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>36000</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12000</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="2">
+        <f>247000+15000</f>
+        <v>262000</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="10">
+        <v>7</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="10">
+        <v>9</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="10">
+        <v>2</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="10">
+        <v>11</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="10">
+        <v>2</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="10">
+        <v>2</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="10">
+        <v>2</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="10">
+        <v>3</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" s="10">
+        <v>4</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="10">
+        <v>4</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="10">
+        <v>9</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="10">
+        <v>2</v>
+      </c>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="10">
+        <v>4</v>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" s="10">
+        <v>2</v>
+      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F32" s="10">
+        <v>1</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="10">
+        <v>1</v>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="10">
+        <v>2</v>
+      </c>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update new firmware. Include: - MotorControl files.
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="178">
   <si>
     <t>Motor 24V</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>Tùm lum thứ</t>
+  </si>
+  <si>
+    <t>Bánh Omni</t>
   </si>
 </sst>
 </file>
@@ -724,6 +727,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -731,12 +740,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1019,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1038,19 +1041,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="2">
         <f>SUM(D5:D47)</f>
-        <v>1768000</v>
+        <v>2878000</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1058,8 +1061,8 @@
         <v>9</v>
       </c>
       <c r="G2" s="2">
-        <f>D5+D6+D7+D8+D12+D14</f>
-        <v>928000</v>
+        <f>D5+D6+D7+D8+D12+D14+D16</f>
+        <v>2038000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1092,7 +1095,7 @@
       </c>
       <c r="G4" s="1">
         <f>G3+G2</f>
-        <v>1768000</v>
+        <v>2878000</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1150,10 +1153,10 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="24">
         <v>4</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1168,8 +1171,8 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1218,10 +1221,10 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="22">
+      <c r="A12" s="24">
         <v>7</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1238,8 +1241,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1276,21 +1279,40 @@
       <c r="A15" s="4">
         <v>9</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="23">
         <v>268000</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>176</v>
       </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <f>370000*3</f>
+        <v>1110000</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Some update in IMU, Encoder, MotorControl, Controller files. Added PID files. Update define.h and include.h for accord.
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="185">
   <si>
     <t>Motor 24V</t>
   </si>
@@ -559,6 +559,27 @@
   </si>
   <si>
     <t>Bánh Omni</t>
+  </si>
+  <si>
+    <t>lần 4</t>
+  </si>
+  <si>
+    <t>Ốc</t>
+  </si>
+  <si>
+    <t>lần 5</t>
+  </si>
+  <si>
+    <t>Keo dán</t>
+  </si>
+  <si>
+    <t>Chuyển nhượng</t>
+  </si>
+  <si>
+    <t>Module cầu H</t>
+  </si>
+  <si>
+    <t>ngày 24/03/2016</t>
   </si>
 </sst>
 </file>
@@ -689,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -740,6 +761,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1022,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1037,10 +1061,11 @@
     <col min="5" max="5" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="18" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
@@ -1053,28 +1078,38 @@
       </c>
       <c r="G1" s="2">
         <f>SUM(D5:D47)</f>
-        <v>2878000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3054000</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="2">
-        <f>D5+D6+D7+D8+D12+D14+D16</f>
-        <v>2038000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <f>D5+D6+D7+D8+D12+D14+D16+D18+H2+D19</f>
+        <v>1602000</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-600000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2">
-        <f>D9+D10+D11+D13+D15</f>
-        <v>840000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="3">
+        <f>D9+D10+D11+D13+D15+D17+H3</f>
+        <v>1452000</v>
+      </c>
+      <c r="H3" s="2">
+        <f>-H2</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1093,12 +1128,12 @@
       <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <f>G3+G2</f>
-        <v>2878000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3054000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1116,7 +1151,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -1134,7 +1169,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -1152,7 +1187,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="24">
         <v>4</v>
       </c>
@@ -1170,7 +1205,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
       <c r="B9" s="25"/>
       <c r="C9" s="2" t="s">
@@ -1184,7 +1219,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -1202,7 +1237,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>6</v>
       </c>
@@ -1220,7 +1255,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
         <v>7</v>
       </c>
@@ -1240,7 +1275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="2" t="s">
@@ -1256,7 +1291,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>8</v>
       </c>
@@ -1275,7 +1310,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>9</v>
       </c>
@@ -1295,7 +1330,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>10</v>
       </c>
@@ -1314,8 +1349,66 @@
       </c>
       <c r="F16" s="2"/>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="24">
+        <v>11</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="2">
+        <v>12000</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="2">
+        <v>14000</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="27">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2">
+        <v>150000</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A1:E1"/>

</xml_diff>